<commit_message>
Adding most recent changes
</commit_message>
<xml_diff>
--- a/src/Config/ControllerNew.xlsx
+++ b/src/Config/ControllerNew.xlsx
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4425" uniqueCount="1055">
   <si>
     <t>TestArea</t>
   </si>
@@ -3337,9 +3337,6 @@
     <t>FPT_URL</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
     <t>FPT Onsite - DAT Practice Test</t>
   </si>
   <si>
@@ -3409,7 +3406,22 @@
     <t>GRE</t>
   </si>
   <si>
-    <t>172.16.219.87:3001</t>
+    <t>172.16.218.192:3001</t>
+  </si>
+  <si>
+    <t>Preview</t>
+  </si>
+  <si>
+    <t>FPT CBT - MCAT Practice Test</t>
+  </si>
+  <si>
+    <t>FPTTC008</t>
+  </si>
+  <si>
+    <t>FPT_CBT_MCAT</t>
+  </si>
+  <si>
+    <t>FPT_CBT</t>
   </si>
 </sst>
 </file>
@@ -3829,7 +3841,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,7 +3889,7 @@
         <v>177</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3901,7 +3913,7 @@
         <v>180</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="2"/>
@@ -3934,11 +3946,11 @@
         <v>1025</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>1026</v>
+        <v>1050</v>
       </c>
       <c r="C8" s="12" t="str">
         <f>IF(B8="QA","http://qwjasweb02.kaplaninc.com/npt.htm",IF(B8="PROD","http://jasper.kaptest.com/npt.htm",IF(B8="Preview","http://preview.kaptest.int.kaplan.com/index.jhtml")))</f>
-        <v>http://qwjasweb02.kaplaninc.com/npt.htm</v>
+        <v>http://preview.kaptest.int.kaplan.com/index.jhtml</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="5"/>
@@ -4246,7 +4258,7 @@
         <v>26</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>21</v>
@@ -4334,7 +4346,7 @@
         <v>26</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>33</v>
@@ -4510,7 +4522,7 @@
         <v>26</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>49</v>
@@ -17567,10 +17579,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -17647,7 +17659,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D2" s="12" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>1020</v>
@@ -17682,7 +17694,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" s="12" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>1020</v>
@@ -17691,7 +17703,7 @@
         <v>1021</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>23</v>
@@ -17712,12 +17724,12 @@
         <v>1020</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D4" s="12" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>1020</v>
@@ -17726,7 +17738,7 @@
         <v>1021</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>23</v>
@@ -17747,12 +17759,12 @@
         <v>1020</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" s="12" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>1020</v>
@@ -17761,7 +17773,7 @@
         <v>1021</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>23</v>
@@ -17782,12 +17794,12 @@
         <v>1020</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D6" s="12" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>1020</v>
@@ -17796,7 +17808,7 @@
         <v>1021</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>23</v>
@@ -17817,12 +17829,12 @@
         <v>1020</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D7" s="12" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>1020</v>
@@ -17831,7 +17843,7 @@
         <v>1021</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>23</v>
@@ -17852,12 +17864,12 @@
         <v>1020</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D8" s="12" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>1020</v>
@@ -17866,7 +17878,7 @@
         <v>1021</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>23</v>
@@ -17878,22 +17890,57 @@
         <v>30</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>642</v>
+        <v>26</v>
       </c>
       <c r="M8" s="12" t="s">
         <v>1020</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>1049</v>
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D9" s="12" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>1053</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>1008</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>1037</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q2"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H9">
       <formula1>"Complete_Regression,Regular_Regression,getQAText"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>